<commit_message>
update project to use tree-based cell type mapping
</commit_message>
<xml_diff>
--- a/tables/color_scales.xlsx
+++ b/tables/color_scales.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="29430" windowHeight="10275" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11370" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="methods" sheetId="1" r:id="rId1"/>
@@ -87,36 +87,6 @@
     <t>backup2</t>
   </si>
   <si>
-    <t>CD4+ T cells</t>
-  </si>
-  <si>
-    <t>CD8+ T cells</t>
-  </si>
-  <si>
-    <t>Natural killer cells</t>
-  </si>
-  <si>
-    <t>Dendritic cells</t>
-  </si>
-  <si>
-    <t>regulatory T cells</t>
-  </si>
-  <si>
-    <t>Macrophages/Monocytes</t>
-  </si>
-  <si>
-    <t>B cells</t>
-  </si>
-  <si>
-    <t>Endothelial cells</t>
-  </si>
-  <si>
-    <t>Cancer associated fibroblasts</t>
-  </si>
-  <si>
-    <t>Other</t>
-  </si>
-  <si>
     <t>value</t>
   </si>
   <si>
@@ -156,10 +126,40 @@
     <t>#ffed6f</t>
   </si>
   <si>
-    <t>Melanoma cells</t>
-  </si>
-  <si>
-    <t>Ovarian carcinoma cells</t>
+    <t>T cell CD8+</t>
+  </si>
+  <si>
+    <t>NK cell</t>
+  </si>
+  <si>
+    <t>Dendritic cell</t>
+  </si>
+  <si>
+    <t>T cell regulatory (Tregs)</t>
+  </si>
+  <si>
+    <t>B cell</t>
+  </si>
+  <si>
+    <t>Endothelial cell</t>
+  </si>
+  <si>
+    <t>Cancer associated fibroblast</t>
+  </si>
+  <si>
+    <t>Melanoma cell</t>
+  </si>
+  <si>
+    <t>Ovarian carcinoma cell</t>
+  </si>
+  <si>
+    <t>other cell</t>
+  </si>
+  <si>
+    <t>Macrophage/Monocyte</t>
+  </si>
+  <si>
+    <t>T cell CD4+ (non-regulatory)</t>
   </si>
 </sst>
 </file>
@@ -525,10 +525,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -613,7 +613,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,87 +623,87 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>1</v>
@@ -711,7 +711,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>0</v>
@@ -719,7 +719,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>10</v>
@@ -730,7 +730,7 @@
         <v>18</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -738,7 +738,7 @@
         <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
improve sensitivity analysis plots
</commit_message>
<xml_diff>
--- a/tables/color_scales.xlsx
+++ b/tables/color_scales.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11370" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010"/>
   </bookViews>
   <sheets>
     <sheet name="methods" sheetId="1" r:id="rId1"/>
     <sheet name="cell_types" sheetId="2" r:id="rId2"/>
+    <sheet name="immune_cells" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="46">
   <si>
     <t>#33a02c</t>
   </si>
@@ -33,30 +34,6 @@
     <t>#e31a1c</t>
   </si>
   <si>
-    <t>#ff7f00</t>
-  </si>
-  <si>
-    <t>#e41a1c</t>
-  </si>
-  <si>
-    <t>#377eb8</t>
-  </si>
-  <si>
-    <t>#4daf4a</t>
-  </si>
-  <si>
-    <t>#984ea3</t>
-  </si>
-  <si>
-    <t>#ffff33</t>
-  </si>
-  <si>
-    <t>#a65628</t>
-  </si>
-  <si>
-    <t>#f781bf</t>
-  </si>
-  <si>
     <t>#999999</t>
   </si>
   <si>
@@ -160,6 +137,33 @@
   </si>
   <si>
     <t>T cell CD4+ (non-regulatory)</t>
+  </si>
+  <si>
+    <t>T cell CD4+</t>
+  </si>
+  <si>
+    <t>#1b9e77</t>
+  </si>
+  <si>
+    <t>#d95f02</t>
+  </si>
+  <si>
+    <t>#7570b3</t>
+  </si>
+  <si>
+    <t>#e7298a</t>
+  </si>
+  <si>
+    <t>#66a61e</t>
+  </si>
+  <si>
+    <t>#e6ab02</t>
+  </si>
+  <si>
+    <t>#a6761d</t>
+  </si>
+  <si>
+    <t>#666666</t>
   </si>
 </sst>
 </file>
@@ -512,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,82 +529,74 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -612,8 +608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,87 +619,87 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>1</v>
@@ -711,7 +707,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>0</v>
@@ -719,26 +715,116 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finish validation analysis and add noise robustness
</commit_message>
<xml_diff>
--- a/tables/color_scales.xlsx
+++ b/tables/color_scales.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11370" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="methods" sheetId="1" r:id="rId1"/>
     <sheet name="cell_types" sheetId="2" r:id="rId2"/>
     <sheet name="immune_cells" sheetId="3" r:id="rId3"/>
+    <sheet name="validation" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="48">
   <si>
     <t>#33a02c</t>
   </si>
@@ -164,6 +165,12 @@
   </si>
   <si>
     <t>#666666</t>
+  </si>
+  <si>
+    <t>Neutrophil</t>
+  </si>
+  <si>
+    <t>T cell</t>
   </si>
 </sst>
 </file>
@@ -518,7 +525,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10:B10"/>
     </sheetView>
   </sheetViews>
@@ -746,8 +753,96 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -813,7 +908,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="B8" t="s">
         <v>44</v>
@@ -821,7 +916,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="B9" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
save figures and results for summary figures.
</commit_message>
<xml_diff>
--- a/tables/color_scales.xlsx
+++ b/tables/color_scales.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11370" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="methods" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="49">
   <si>
     <t>#33a02c</t>
   </si>
@@ -171,6 +171,9 @@
   </si>
   <si>
     <t>T cell</t>
+  </si>
+  <si>
+    <t>PBMC</t>
   </si>
 </sst>
 </file>
@@ -613,10 +616,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -653,7 +656,7 @@
         <v>26</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -725,22 +728,30 @@
         <v>34</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>11</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>23</v>
       </c>
     </row>
@@ -841,7 +852,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
build migration charts in spillover analysis
</commit_message>
<xml_diff>
--- a/tables/color_scales.xlsx
+++ b/tables/color_scales.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="methods" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="52">
   <si>
     <t>#33a02c</t>
   </si>
@@ -174,6 +174,15 @@
   </si>
   <si>
     <t>PBMC</t>
+  </si>
+  <si>
+    <t>Macrophage M1</t>
+  </si>
+  <si>
+    <t>Macrophage M2</t>
+  </si>
+  <si>
+    <t>Monocyte</t>
   </si>
 </sst>
 </file>
@@ -618,7 +627,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -762,9 +771,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -841,6 +852,30 @@
       </c>
       <c r="B9" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
improve tcga comparison figure
</commit_message>
<xml_diff>
--- a/tables/color_scales.xlsx
+++ b/tables/color_scales.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\projects\immune_deconvolution_benchmark\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{63B4D583-8064-4570-96CA-F4E005840C3D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="methods" sheetId="1" r:id="rId1"/>
     <sheet name="cell_types" sheetId="2" r:id="rId2"/>
-    <sheet name="immune_cells" sheetId="3" r:id="rId3"/>
-    <sheet name="validation" sheetId="4" r:id="rId4"/>
+    <sheet name="cell_types_for_tcga" sheetId="5" r:id="rId3"/>
+    <sheet name="immune_cells" sheetId="3" r:id="rId4"/>
+    <sheet name="validation" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="54">
   <si>
     <t>#33a02c</t>
   </si>
@@ -183,12 +185,18 @@
   </si>
   <si>
     <t>Monocyte</t>
+  </si>
+  <si>
+    <t>Macrophage</t>
+  </si>
+  <si>
+    <t>Eosinophil</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -534,7 +542,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -624,7 +632,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -770,11 +778,142 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07ED3994-7B7D-4372-AB6F-1716A6625F61}">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -883,8 +1022,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
add 10th value to color palette
</commit_message>
<xml_diff>
--- a/tables/color_scales.xlsx
+++ b/tables/color_scales.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="64">
   <si>
     <t xml:space="preserve">value</t>
   </si>
@@ -189,28 +189,34 @@
     <t xml:space="preserve">T cell</t>
   </si>
   <si>
-    <t xml:space="preserve">#e41a1c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#377eb8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#4daf4a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#984ea3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#ff7f00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#ffff33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#a65628</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#f781bf</t>
+    <t xml:space="preserve">#1f77b4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#ff7f0e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#2ca02c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#d62728</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#9467bd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#8c564b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#e377c2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#7f7f7f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#bcbd22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#17becf</t>
   </si>
 </sst>
 </file>
@@ -286,13 +292,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -927,7 +937,7 @@
   <dimension ref="A1:D44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -944,11 +954,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="2" t="s">
         <v>54</v>
       </c>
     </row>
@@ -960,60 +970,68 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="0" t="s">
-        <v>43</v>
+      <c r="B10" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>